<commit_message>
Added solve_pH and rMatrix section
Implemented solve_pH, which solved the pH based on a Newton-Raphson to find the root of the charge balance.
Also implemented rMatrix_section, which calculates the reaction matrix for a certain region. This matrix contains the concentration changes [mol/h] for each compound for each gridcell
</commit_message>
<xml_diff>
--- a/planning/test_file.xlsx
+++ b/planning/test_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568C1AE1-81D2-4D75-BA16-5E171ACE14CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E33896-CB7D-48B2-9F3B-AC508D3CD9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -9563,7 +9563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -9864,8 +9864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented tests and bug fixes
Implemented tests for the reaction_matrix files and fixed bugs in those files
</commit_message>
<xml_diff>
--- a/planning/test_file.xlsx
+++ b/planning/test_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E33896-CB7D-48B2-9F3B-AC508D3CD9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A8FAEF-7C4C-4590-BF17-969DE5D14296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="808" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="808" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -1336,18 +1336,12 @@
     <t>Average expected radius of all granules</t>
   </si>
   <si>
-    <t>density granule</t>
-  </si>
-  <si>
     <t>g/L</t>
   </si>
   <si>
     <t>How dense are the granules</t>
   </si>
   <si>
-    <t>density reactor</t>
-  </si>
-  <si>
     <t>How much biomass (at most) is in the reactor</t>
   </si>
   <si>
@@ -1409,6 +1403,12 @@
   </si>
   <si>
     <t>suspension</t>
+  </si>
+  <si>
+    <t>Density granule</t>
+  </si>
+  <si>
+    <t>Density reactor</t>
   </si>
 </sst>
 </file>
@@ -4285,7 +4285,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B1" s="121">
         <f>Influent!B1/2</f>
@@ -4303,7 +4303,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B2" s="121">
         <f>Influent!B2/2</f>
@@ -4461,7 +4461,7 @@
     </row>
     <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B2" s="151" t="s">
         <v>85</v>
@@ -4490,7 +4490,7 @@
     </row>
     <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B3" s="151" t="s">
         <v>85</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="13" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="76" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B13" s="103">
         <f>IF(COUNT(B2,C2)=2, EXP(($C$10+B2-C2)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
@@ -4776,7 +4776,7 @@
     </row>
     <row r="14" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B14" s="103">
         <f>IF(COUNT(B3,C3)=2, EXP(($C$10+B3-C3)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
@@ -4992,7 +4992,7 @@
     </row>
     <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B24" s="152" t="s">
         <v>86</v>
@@ -5015,7 +5015,7 @@
     </row>
     <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B25" s="152" t="s">
         <v>86</v>
@@ -5269,10 +5269,10 @@
     <row r="1" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
       <c r="B1" s="136" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C1" s="136" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D1" s="136" t="s">
         <v>17</v>
@@ -5281,12 +5281,12 @@
         <v>76</v>
       </c>
       <c r="F1" s="275" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B2" s="100">
         <v>1.0000000000000001E-5</v>
@@ -5304,7 +5304,7 @@
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B3" s="100">
         <v>0</v>
@@ -5322,7 +5322,7 @@
     </row>
     <row r="4" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B4" s="100">
         <v>0</v>
@@ -5376,21 +5376,21 @@
     <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
       <c r="B1" s="136" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C1" s="136" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D1" s="136" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="275" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B2" s="100">
         <v>0</v>
@@ -5405,7 +5405,7 @@
     </row>
     <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B3" s="100">
         <v>0</v>
@@ -5420,7 +5420,7 @@
     </row>
     <row r="4" spans="1:5" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B4" s="100">
         <v>0</v>
@@ -5478,18 +5478,18 @@
         <v>225</v>
       </c>
       <c r="F1" s="270" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B2" s="100">
         <v>0.01</v>
       </c>
       <c r="C2" s="137" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D2" s="138">
         <f>0.25/24</f>
@@ -5503,13 +5503,13 @@
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B3" s="100">
         <v>0.01</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D3" s="138">
         <f>0.25/24</f>
@@ -5523,7 +5523,7 @@
     </row>
     <row r="4" spans="1:6" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B4" s="100">
         <v>0.01</v>
@@ -5574,17 +5574,17 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
       <c r="B1" s="276" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C1" s="277"/>
       <c r="D1" s="278"/>
       <c r="E1" s="276" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F1" s="277"/>
       <c r="G1" s="278"/>
       <c r="H1" s="277" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I1" s="277"/>
       <c r="J1" s="278"/>
@@ -5621,7 +5621,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="76" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B3" s="164">
         <v>-1</v>
@@ -5653,7 +5653,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B4" s="166">
         <v>0</v>
@@ -8612,8 +8612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8676,7 +8676,7 @@
         <v>161</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C4" s="119" t="s">
         <v>90</v>
@@ -8780,31 +8780,31 @@
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="B11" s="225">
         <v>100</v>
       </c>
       <c r="C11" s="90" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" s="226" t="s">
         <v>254</v>
-      </c>
-      <c r="D11" s="226" t="s">
-        <v>255</v>
       </c>
       <c r="E11" s="69"/>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="89" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="B12" s="227">
         <v>3</v>
       </c>
       <c r="C12" s="92" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12" s="228" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E12" s="69"/>
     </row>
@@ -9219,7 +9219,7 @@
         <v>90</v>
       </c>
       <c r="D18" s="107" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E18" s="264"/>
     </row>
@@ -9337,10 +9337,10 @@
         <v>0.2</v>
       </c>
       <c r="C26" s="90" t="s">
+        <v>262</v>
+      </c>
+      <c r="D26" s="112" t="s">
         <v>264</v>
-      </c>
-      <c r="D26" s="112" t="s">
-        <v>266</v>
       </c>
       <c r="E26" s="264"/>
     </row>
@@ -9352,10 +9352,10 @@
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="C27" s="90" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D27" s="112" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E27" s="264"/>
     </row>
@@ -9417,7 +9417,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B1" s="116">
         <f>1*10^(-9)*3600</f>
@@ -9435,7 +9435,7 @@
     </row>
     <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B2" s="116">
         <f>1*10^(-9)*3600</f>
@@ -9656,13 +9656,13 @@
         <v>200</v>
       </c>
       <c r="B6" s="184" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C6" s="129" t="s">
         <v>90</v>
       </c>
       <c r="D6" s="232" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -9697,7 +9697,7 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="174" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B9" s="122">
         <v>12</v>
@@ -9706,12 +9706,12 @@
         <v>90</v>
       </c>
       <c r="D9" s="233" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="234" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B10" s="186">
         <v>12</v>
@@ -9720,7 +9720,7 @@
         <v>90</v>
       </c>
       <c r="D10" s="235" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -9770,7 +9770,7 @@
         <v>187</v>
       </c>
       <c r="B14" s="128" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C14" s="129" t="s">
         <v>90</v>
@@ -9864,8 +9864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9966,10 +9966,10 @@
         <v>0.05</v>
       </c>
       <c r="C7" s="90" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D7" s="231" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -10087,7 +10087,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B1" s="121">
         <f>2*Parameters!B3</f>
@@ -10110,7 +10110,7 @@
     </row>
     <row r="2" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B2" s="121">
         <f>2*Parameters!B3</f>

</xml_diff>